<commit_message>
update lijngericht weer toevoegen
</commit_message>
<xml_diff>
--- a/werkafspraken/bag 2.0/media/BAG-BGT werkinstructie v0.4.xlsx
+++ b/werkafspraken/bag 2.0/media/BAG-BGT werkinstructie v0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\GitHub\Geonovum\IMGeo\werkafspraken\bag 2.0\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7920570A-8193-4CF4-A726-E9F41C06B920}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5497D6E3-F837-4ED8-B358-4E4DA9424C56}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +344,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -353,11 +359,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -365,24 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -392,14 +395,47 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A45" sqref="A2:F45"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,684 +768,738 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="10">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="10">
         <v>1</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="13" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="10">
         <v>1</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="15"/>
+      <c r="B31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="10">
         <v>1</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="A34" s="16"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="5">
+      <c r="F34" s="13"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="10">
         <v>2</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="A36" s="16"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6" t="s">
+      <c r="F36" s="13"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="A38" s="16"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="5" t="s">
+      <c r="F38" s="13"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
+      <c r="B39" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="A40" s="16"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="5" t="s">
+      <c r="F40" s="13"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
+      <c r="B41" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="A42" s="16"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="14"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="5"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="5"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
+      <c r="A46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
+      <c r="A47" s="5"/>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
+      <c r="A48" s="5"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
+      <c r="A49" s="5"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11"/>
+      <c r="A50" s="5"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
+      <c r="A51" s="5"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
+      <c r="A52" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="52">
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="F9:F13"/>
     <mergeCell ref="F15:F19"/>

</xml_diff>